<commit_message>
feat: enhance create-multiple page with QR code generation and improved file handling, page for view attestation
</commit_message>
<xml_diff>
--- a/public/diploma.xlsx
+++ b/public/diploma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\belowevolve\learning\eas-diploma\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B4B36B-D81D-45ED-8C03-8C6BA7D70094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6794CAAD-5883-4AB4-A350-0E9D905F3372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Разработка блокчейн-приложений</t>
   </si>
   <si>
-    <t>0x1234567890123456789012345678901234567890</t>
-  </si>
-  <si>
     <t>Бакалавр</t>
   </si>
   <si>
@@ -81,7 +78,10 @@
     <t>Экономические модели в блокчейне</t>
   </si>
   <si>
-    <t xml:space="preserve">0x2345678901234567890123456789012345678901 </t>
+    <t>0x7CE2cfC2b3c838150d110cF78d156d96674afe54</t>
+  </si>
+  <si>
+    <t>0x04628CC763C09e41aDC9C6b6F28ED7d6c35d7d42</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,24 +450,24 @@
         <v>2024</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
       <c r="F3">
         <v>2024</v>

</xml_diff>

<commit_message>
chore: ui and lang improvements
</commit_message>
<xml_diff>
--- a/public/diploma.xlsx
+++ b/public/diploma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\belowevolve\learning\eas-diploma\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6794CAAD-5883-4AB4-A350-0E9D905F3372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C1EA43-8B08-4354-9CF4-22BE15859F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>degree</t>
   </si>
@@ -54,47 +54,145 @@
     <t>Иванов Иван Иванович</t>
   </si>
   <si>
-    <t>Информатика</t>
-  </si>
-  <si>
-    <t>Компьютерные науки</t>
-  </si>
-  <si>
-    <t>Разработка блокчейн-приложений</t>
-  </si>
-  <si>
     <t>Бакалавр</t>
   </si>
   <si>
     <t>Петров Петр Петрович</t>
   </si>
   <si>
-    <t>Экономика</t>
-  </si>
-  <si>
-    <t>Финансы</t>
-  </si>
-  <si>
-    <t>Экономические модели в блокчейне</t>
-  </si>
-  <si>
     <t>0x7CE2cfC2b3c838150d110cF78d156d96674afe54</t>
   </si>
   <si>
     <t>0x04628CC763C09e41aDC9C6b6F28ED7d6c35d7d42</t>
+  </si>
+  <si>
+    <t>Разработка адаптивной системы управления сложным техническим объектом</t>
+  </si>
+  <si>
+    <t>Разработка адаптера блокчейна Tron для существующей криптовалютной биржи</t>
+  </si>
+  <si>
+    <t>Система автоматического формирования метеопредупреждений на основе прогнозирования показаний метеостанции</t>
+  </si>
+  <si>
+    <t>Модели и алгоритмы оценивания технического состояния сложных технических объектов на основе стохастических моделей</t>
+  </si>
+  <si>
+    <t>Оптимизация управления производством программных проектов</t>
+  </si>
+  <si>
+    <t>Программная инженерия</t>
+  </si>
+  <si>
+    <t>Институт информационных технологий и программирования</t>
+  </si>
+  <si>
+    <t>Разработка веб-приложения для рейтингового учета результатов игр "Спортивная мафия"</t>
+  </si>
+  <si>
+    <t>Разработка программного модуля процедурной генерации игровых уровней</t>
+  </si>
+  <si>
+    <t>Разработка высоконагруженной отказоустойчивой системы SMS-оповещения в чрезвычайных ситуациях</t>
+  </si>
+  <si>
+    <t>Приложение для изучения адресации стека протокола TPC/IP v.6</t>
+  </si>
+  <si>
+    <t>Исследование и оптимизация пользовательского интерфейса Blender для улучшения процесса 3D моделирования</t>
+  </si>
+  <si>
+    <t>Фролов Иван Никитич</t>
+  </si>
+  <si>
+    <t>Степанова Мария Владиславовна</t>
+  </si>
+  <si>
+    <t>Богомолов Тимофей Андреевич</t>
+  </si>
+  <si>
+    <t>Поляков Матвей Львович</t>
+  </si>
+  <si>
+    <t>Терентьева Агата Михайловна</t>
+  </si>
+  <si>
+    <t>Муравьев Виктор Тимофеевич</t>
+  </si>
+  <si>
+    <t>Королева Ярослава Никитична</t>
+  </si>
+  <si>
+    <t>Грачев Максим Матвеевич</t>
+  </si>
+  <si>
+    <t>0xeb7a92cfc24d7207c9df0631e15a13c576c187a4</t>
+  </si>
+  <si>
+    <t>0xf8ed978fe59f2fafa4a31776bec6a345efef609e</t>
+  </si>
+  <si>
+    <t>0x5acc2e76f1efcd41d4925235894cd7822903c207</t>
+  </si>
+  <si>
+    <t>0xb02c1b0c2f2776b9c824b9635886f9fc92956cb3</t>
+  </si>
+  <si>
+    <t>0x4b029d34371fc77d730fe8c2bf4f051eb12ede17</t>
+  </si>
+  <si>
+    <t>0xd769aa389424952c8f151499034bba519ef7cbaf</t>
+  </si>
+  <si>
+    <t>0x3ff3a73c63264654e0bea5453c2595880204b37b</t>
+  </si>
+  <si>
+    <t>0x9bbac0b8029710f7e9e0a489a65978a490e83a25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Cyr"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -113,15 +211,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 14" xfId="6" xr:uid="{4040B32B-67B9-49FF-85BD-2F5327DEA22E}"/>
+    <cellStyle name="Обычный 16" xfId="3" xr:uid="{5AB0B527-0276-4BC2-B4BA-27001BD24C98}"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{D3FA5EEC-A1F8-47BA-989D-8FB2778F9D10}"/>
+    <cellStyle name="Обычный 2 2" xfId="2" xr:uid="{22FFE7EA-B62B-4595-8E3F-75B3C14481BB}"/>
+    <cellStyle name="Обычный 3" xfId="4" xr:uid="{D7A776E4-05AE-4EFD-9A64-17A364CD8776}"/>
+    <cellStyle name="Обычный 3 2" xfId="8" xr:uid="{EAAB94EA-DE9E-4C4C-BF19-4A3055D185E7}"/>
+    <cellStyle name="Обычный 4" xfId="5" xr:uid="{374EDF9E-7DBD-4F4D-8611-878D1E769D50}"/>
+    <cellStyle name="Обычный 5" xfId="7" xr:uid="{C873CC8A-0E8F-4899-A55A-2330EB4BC461}"/>
+    <cellStyle name="Обычный 5 2" xfId="9" xr:uid="{3C2AFA97-4073-40B9-BD7B-39E9EF5F1F3D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -399,13 +565,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -430,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -438,42 +609,226 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>2024</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2024</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>2024</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <v>2024</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: better date in attestation
</commit_message>
<xml_diff>
--- a/public/diploma.xlsx
+++ b/public/diploma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\belowevolve\learning\eas-diploma\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C1EA43-8B08-4354-9CF4-22BE15859F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6246E53F-2D92-4A67-839B-DD4D3E06A3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -276,6 +276,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -568,7 +569,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,6 +577,7 @@
     <col min="3" max="3" width="17.54296875" customWidth="1"/>
     <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78.90625" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -617,8 +619,8 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2">
-        <v>2024</v>
+      <c r="F2" s="6">
+        <v>45467</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -640,8 +642,8 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
-        <v>2024</v>
+      <c r="F3" s="6">
+        <v>45467</v>
       </c>
       <c r="G3" t="s">
         <v>12</v>
@@ -663,14 +665,14 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1">
-        <v>2024</v>
+      <c r="F4" s="6">
+        <v>45467</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -686,14 +688,14 @@
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1">
-        <v>2024</v>
+      <c r="F5" s="6">
+        <v>45467</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -709,14 +711,14 @@
       <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1">
-        <v>2024</v>
+      <c r="F6" s="6">
+        <v>45467</v>
       </c>
       <c r="G6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -732,14 +734,14 @@
       <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1">
-        <v>2024</v>
+      <c r="F7" s="6">
+        <v>45467</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -755,14 +757,14 @@
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1">
-        <v>2024</v>
+      <c r="F8" s="6">
+        <v>45467</v>
       </c>
       <c r="G8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -778,14 +780,14 @@
       <c r="E9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1">
-        <v>2024</v>
+      <c r="F9" s="6">
+        <v>45467</v>
       </c>
       <c r="G9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -801,14 +803,14 @@
       <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1">
-        <v>2024</v>
+      <c r="F10" s="6">
+        <v>45467</v>
       </c>
       <c r="G10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -824,8 +826,8 @@
       <c r="E11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1">
-        <v>2024</v>
+      <c r="F11" s="6">
+        <v>45467</v>
       </c>
       <c r="G11" t="s">
         <v>40</v>

</xml_diff>